<commit_message>
testeando cambios de excel
</commit_message>
<xml_diff>
--- a/ADA1/ADA1.xlsx
+++ b/ADA1/ADA1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2831083-CF65-4380-86FA-3B76D491B809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1DAB91-1D6C-4418-B72F-565944AD8472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Computing Essentials</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>Diseño de Bases de Datos</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -635,44 +638,44 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,7 +995,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,10 +1029,10 @@
       <c r="H1" s="26"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="34">
         <v>152</v>
       </c>
       <c r="D2" s="21" t="s">
@@ -1038,7 +1041,7 @@
       <c r="E2" s="22">
         <v>56</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="41">
         <f>SUM(E2:E12)</f>
         <v>378</v>
       </c>
@@ -1046,15 +1049,15 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E3" s="8">
         <v>40</v>
       </c>
-      <c r="F3" s="33"/>
+      <c r="F3" s="42"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -1064,15 +1067,15 @@
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="43"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="8">
         <v>40</v>
       </c>
-      <c r="F4" s="33"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1082,104 +1085,106 @@
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="43"/>
-      <c r="C5" s="41"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E5" s="13">
         <v>46</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="44" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="32" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="13"/>
-      <c r="F6" s="33"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="44" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="32" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="13">
         <v>60</v>
       </c>
-      <c r="F7" s="33"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
-      <c r="C8" s="41"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="13">
         <v>28</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="43"/>
-      <c r="C9" s="41"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="12" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="13">
         <v>40</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="41"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="13">
         <v>68</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="12"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="33"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="43"/>
-      <c r="C12" s="41"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="33"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="35">
         <v>80</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -1188,7 +1193,7 @@
       <c r="E13" s="19">
         <v>40</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="41">
         <f>SUM(E13:E28)</f>
         <v>690</v>
       </c>
@@ -1196,193 +1201,193 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="37"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="16" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="17">
         <v>32</v>
       </c>
-      <c r="F14" s="33"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
-      <c r="C15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="16" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="17">
         <v>64</v>
       </c>
-      <c r="F15" s="33"/>
+      <c r="F15" s="42"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="35"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="16" t="s">
         <v>34</v>
       </c>
       <c r="E16" s="17">
         <v>40</v>
       </c>
-      <c r="F16" s="33"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="35"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="44" t="s">
+      <c r="B17" s="38"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="32" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="17">
         <v>64</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="42"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="35"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="44" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="32" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="17">
         <v>72</v>
       </c>
-      <c r="F18" s="33"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="44" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="32" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="17">
         <v>72</v>
       </c>
-      <c r="F19" s="33"/>
+      <c r="F19" s="42"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="35"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="44" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="32" t="s">
         <v>69</v>
       </c>
       <c r="E20" s="17">
         <v>72</v>
       </c>
-      <c r="F20" s="33"/>
+      <c r="F20" s="42"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="35"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="44" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="32" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="17">
         <v>64</v>
       </c>
-      <c r="F21" s="33"/>
+      <c r="F21" s="42"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="16" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="17">
         <v>20</v>
       </c>
-      <c r="F22" s="33"/>
+      <c r="F22" s="42"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="17">
         <v>20</v>
       </c>
-      <c r="F23" s="33"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="35"/>
-      <c r="C24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="16"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="33"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="35"/>
-      <c r="C25" s="37"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="16"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="33"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="35"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="16"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="33"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="35"/>
-      <c r="C27" s="37"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E27" s="17">
         <v>62</v>
       </c>
-      <c r="F27" s="33"/>
+      <c r="F27" s="42"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="35"/>
-      <c r="C28" s="37"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E28" s="17">
         <v>68</v>
       </c>
-      <c r="F28" s="33"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="34">
         <v>29</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1391,7 +1396,7 @@
       <c r="E29" s="22">
         <v>48</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="41">
         <f>SUM(E29:E32)</f>
         <v>552</v>
       </c>
@@ -1399,49 +1404,49 @@
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="43"/>
-      <c r="C30" s="41"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="34"/>
       <c r="D30" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E30" s="13">
         <v>480</v>
       </c>
-      <c r="F30" s="33"/>
+      <c r="F30" s="42"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="41"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34"/>
       <c r="D31" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E31" s="13">
         <v>0</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="42"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="43"/>
-      <c r="C32" s="41"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
       <c r="D32" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="13">
         <v>24</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="2:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="36">
         <v>28</v>
       </c>
       <c r="D33" s="14" t="s">
@@ -1450,7 +1455,7 @@
       <c r="E33" s="15">
         <v>32</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="43">
         <f>SUM(E33:E39)</f>
         <v>112</v>
       </c>
@@ -1458,79 +1463,79 @@
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="35"/>
-      <c r="C34" s="37"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="36"/>
       <c r="D34" s="16" t="s">
         <v>39</v>
       </c>
       <c r="E34" s="17">
         <v>20</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="44"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="35"/>
-      <c r="C35" s="37"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E35" s="17">
         <v>60</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="44"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="35"/>
-      <c r="C36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="16"/>
       <c r="E36" s="17"/>
-      <c r="F36" s="39"/>
+      <c r="F36" s="44"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="35"/>
-      <c r="C37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="16"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="39"/>
+      <c r="F37" s="44"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="35"/>
-      <c r="C38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="16"/>
       <c r="E38" s="17"/>
-      <c r="F38" s="39"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="35"/>
-      <c r="C39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="16"/>
       <c r="E39" s="17"/>
-      <c r="F39" s="39"/>
+      <c r="F39" s="44"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="2:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="40">
+      <c r="C40" s="39">
         <v>30</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="11"/>
-      <c r="F40" s="32">
+      <c r="F40" s="41">
         <f>SUM(E40:E43)</f>
         <v>0</v>
       </c>
@@ -1538,37 +1543,37 @@
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="43"/>
-      <c r="C41" s="41"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
       <c r="D41" s="12"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="33"/>
+      <c r="F41" s="42"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="43"/>
-      <c r="C42" s="41"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="34"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="33"/>
+      <c r="F42" s="42"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="43"/>
-      <c r="C43" s="41"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="34"/>
       <c r="D43" s="12"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="33"/>
+      <c r="F43" s="42"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="37">
+      <c r="C44" s="36">
         <v>48</v>
       </c>
       <c r="D44" s="14" t="s">
@@ -1577,7 +1582,7 @@
       <c r="E44" s="15">
         <v>40</v>
       </c>
-      <c r="F44" s="38">
+      <c r="F44" s="43">
         <f>SUM(E44:E48)</f>
         <v>162</v>
       </c>
@@ -1585,56 +1590,56 @@
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="35"/>
-      <c r="C45" s="37"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E45" s="17">
         <v>68</v>
       </c>
-      <c r="F45" s="39"/>
+      <c r="F45" s="44"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="35"/>
-      <c r="C46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="16" t="s">
         <v>75</v>
       </c>
       <c r="E46" s="17">
         <v>54</v>
       </c>
-      <c r="F46" s="39"/>
+      <c r="F46" s="44"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="35"/>
-      <c r="C47" s="37"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="36"/>
       <c r="D47" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E47" s="17"/>
-      <c r="F47" s="39"/>
+      <c r="F47" s="44"/>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
     <row r="48" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="35"/>
-      <c r="C48" s="37"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="36"/>
       <c r="D48" s="16"/>
       <c r="E48" s="17"/>
-      <c r="F48" s="39"/>
+      <c r="F48" s="44"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="2:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="40">
+      <c r="C49" s="39">
         <v>37</v>
       </c>
       <c r="D49" s="10" t="s">
@@ -1643,7 +1648,7 @@
       <c r="E49" s="11">
         <v>32</v>
       </c>
-      <c r="F49" s="32">
+      <c r="F49" s="41">
         <f>SUM(E49:E54)</f>
         <v>32</v>
       </c>
@@ -1651,55 +1656,55 @@
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="43"/>
-      <c r="C50" s="41"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
       <c r="D50" s="12"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="33"/>
+      <c r="F50" s="42"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="43"/>
-      <c r="C51" s="41"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="34"/>
       <c r="D51" s="12"/>
       <c r="E51" s="13"/>
-      <c r="F51" s="33"/>
+      <c r="F51" s="42"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="43"/>
-      <c r="C52" s="41"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="34"/>
       <c r="D52" s="12"/>
       <c r="E52" s="13"/>
-      <c r="F52" s="33"/>
+      <c r="F52" s="42"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="43"/>
-      <c r="C53" s="41"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
       <c r="D53" s="12"/>
       <c r="E53" s="13"/>
-      <c r="F53" s="33"/>
+      <c r="F53" s="42"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
     </row>
     <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="43"/>
-      <c r="C54" s="41"/>
+      <c r="B54" s="33"/>
+      <c r="C54" s="34"/>
       <c r="D54" s="12"/>
       <c r="E54" s="13"/>
-      <c r="F54" s="33"/>
+      <c r="F54" s="42"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="37">
+      <c r="C55" s="36">
         <v>33</v>
       </c>
       <c r="D55" s="14" t="s">
@@ -1708,7 +1713,7 @@
       <c r="E55" s="15">
         <v>32</v>
       </c>
-      <c r="F55" s="38">
+      <c r="F55" s="43">
         <f>SUM(E55:E60)</f>
         <v>152</v>
       </c>
@@ -1716,63 +1721,63 @@
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="35"/>
-      <c r="C56" s="37"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="36"/>
       <c r="D56" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E56" s="17">
         <v>72</v>
       </c>
-      <c r="F56" s="39"/>
+      <c r="F56" s="44"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="35"/>
-      <c r="C57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="36"/>
       <c r="D57" s="16" t="s">
         <v>67</v>
       </c>
       <c r="E57" s="17">
         <v>48</v>
       </c>
-      <c r="F57" s="39"/>
+      <c r="F57" s="44"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="35"/>
-      <c r="C58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="16"/>
       <c r="E58" s="17"/>
-      <c r="F58" s="39"/>
+      <c r="F58" s="44"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="35"/>
-      <c r="C59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="16"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="39"/>
+      <c r="F59" s="44"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="35"/>
-      <c r="C60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="16"/>
       <c r="E60" s="17"/>
-      <c r="F60" s="39"/>
+      <c r="F60" s="44"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="42" t="s">
+      <c r="B61" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="40">
+      <c r="C61" s="39">
         <v>10</v>
       </c>
       <c r="D61" s="10" t="s">
@@ -1781,7 +1786,7 @@
       <c r="E61" s="11">
         <v>68</v>
       </c>
-      <c r="F61" s="32">
+      <c r="F61" s="41">
         <f>SUM(E61:E65)</f>
         <v>68</v>
       </c>
@@ -1789,46 +1794,46 @@
       <c r="H61" s="7"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="43"/>
-      <c r="C62" s="41"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="34"/>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
-      <c r="F62" s="33"/>
+      <c r="F62" s="42"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="43"/>
-      <c r="C63" s="41"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="34"/>
       <c r="D63" s="12"/>
       <c r="E63" s="13"/>
-      <c r="F63" s="33"/>
+      <c r="F63" s="42"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="43"/>
-      <c r="C64" s="41"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="34"/>
       <c r="D64" s="12"/>
       <c r="E64" s="13"/>
-      <c r="F64" s="33"/>
+      <c r="F64" s="42"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
     </row>
     <row r="65" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="43"/>
-      <c r="C65" s="41"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
       <c r="D65" s="12"/>
       <c r="E65" s="13"/>
-      <c r="F65" s="33"/>
+      <c r="F65" s="42"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="36">
+      <c r="C66" s="35">
         <v>20</v>
       </c>
       <c r="D66" s="18" t="s">
@@ -1837,7 +1842,7 @@
       <c r="E66" s="19">
         <v>20</v>
       </c>
-      <c r="F66" s="38">
+      <c r="F66" s="43">
         <f>SUM(E66:E70)</f>
         <v>20</v>
       </c>
@@ -1845,57 +1850,43 @@
       <c r="H66" s="7"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="35"/>
-      <c r="C67" s="37"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="36"/>
       <c r="D67" s="16"/>
       <c r="E67" s="17"/>
-      <c r="F67" s="39"/>
+      <c r="F67" s="44"/>
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="35"/>
-      <c r="C68" s="37"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="36"/>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>
-      <c r="F68" s="39"/>
+      <c r="F68" s="44"/>
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="35"/>
-      <c r="C69" s="37"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="36"/>
       <c r="D69" s="16"/>
       <c r="E69" s="17"/>
-      <c r="F69" s="39"/>
+      <c r="F69" s="44"/>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="35"/>
-      <c r="C70" s="37"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="36"/>
       <c r="D70" s="16"/>
       <c r="E70" s="17"/>
-      <c r="F70" s="39"/>
+      <c r="F70" s="44"/>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C12"/>
-    <mergeCell ref="C13:C28"/>
-    <mergeCell ref="B13:B28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C44:C48"/>
-    <mergeCell ref="B44:B48"/>
     <mergeCell ref="F13:F28"/>
     <mergeCell ref="F29:F32"/>
     <mergeCell ref="B66:B70"/>
@@ -1912,6 +1903,20 @@
     <mergeCell ref="B49:B54"/>
     <mergeCell ref="C55:C60"/>
     <mergeCell ref="B55:B60"/>
+    <mergeCell ref="C61:C65"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C44:C48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C2:C12"/>
+    <mergeCell ref="C13:C28"/>
+    <mergeCell ref="B13:B28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="B29:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2686,6 +2691,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100320CD0579582C4469834566D7EA084A0" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1aca7042d47997f19315c281147fbd7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca1a50c8-878d-40f3-95c4-2166ee7c49e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71c039766ad27feaa2f90db93a82ba51" ns2:_="">
     <xsd:import namespace="ca1a50c8-878d-40f3-95c4-2166ee7c49e1"/>
@@ -2817,22 +2837,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A990CFAD-EFFD-4C9C-99EF-ACD68CE62B3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ca1a50c8-878d-40f3-95c4-2166ee7c49e1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBAAD37E-BE7C-4046-AF99-E5AF0FD26725}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBFCAEE0-E841-4A11-82F1-DBDEFB2F24FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2848,28 +2877,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBAAD37E-BE7C-4046-AF99-E5AF0FD26725}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A990CFAD-EFFD-4C9C-99EF-ACD68CE62B3C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ca1a50c8-878d-40f3-95c4-2166ee7c49e1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>